<commit_message>
versão sem implementação de rubricas
</commit_message>
<xml_diff>
--- a/resultado_progressao.xlsx
+++ b/resultado_progressao.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -522,7 +522,7 @@
         <v>6</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>1339</v>
+        <v>1339.26</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -530,6 +530,47 @@
         </is>
       </c>
       <c r="I2" t="inlineStr">
+        <is>
+          <t>407 DE 03/11/2025 PROGESP</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>342456</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Thiago Aparecido Nogueira Basso</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Novembro2025</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>00001</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>r</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>6</v>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>232.2</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>406 DE 03/11/2025 PROGESP</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
         <is>
           <t>407 DE 03/11/2025 PROGESP</t>
         </is>

</xml_diff>